<commit_message>
Updated Exports.xlsx with new data
</commit_message>
<xml_diff>
--- a/Exports.xlsx
+++ b/Exports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bentleyedu-my.sharepoint.com/personal/fcastagliuolo_falcon_bentley_edu/Documents/GitHubPython/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bentleyedu-my.sharepoint.com/personal/fcastagliuolo_falcon_bentley_edu/Documents/NECBL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="663" documentId="8_{CFF33F4F-308C-41CB-8120-A7DBF34109D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6F0B417-9761-40CE-93CB-503D592FCCA6}"/>
+  <xr:revisionPtr revIDLastSave="686" documentId="8_{CFF33F4F-308C-41CB-8120-A7DBF34109D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3CE01B6-8353-43BE-96B0-368FDABCB082}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="1116" windowWidth="21624" windowHeight="11052" firstSheet="4" activeTab="8" xr2:uid="{749FCA05-89A3-4D1F-A8C9-25177A9E2D98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{749FCA05-89A3-4D1F-A8C9-25177A9E2D98}"/>
   </bookViews>
   <sheets>
     <sheet name="xWA" sheetId="1" r:id="rId1"/>
@@ -8138,6 +8138,54 @@
           <cell r="L46">
             <v>1.4076116324469214</v>
           </cell>
+          <cell r="S46">
+            <v>0.475724881892711</v>
+          </cell>
+          <cell r="T46">
+            <v>0.15857496063090368</v>
+          </cell>
+          <cell r="U46">
+            <v>0.93188675055421044</v>
+          </cell>
+          <cell r="V46">
+            <v>1.090461711185114</v>
+          </cell>
+          <cell r="W46">
+            <v>1.090461711185114</v>
+          </cell>
+          <cell r="X46">
+            <v>1.2490366718160177</v>
+          </cell>
+          <cell r="Y46">
+            <v>1.2490366718160177</v>
+          </cell>
+          <cell r="Z46">
+            <v>1.4076116324469214</v>
+          </cell>
+          <cell r="AA46">
+            <v>0.39400587846154067</v>
+          </cell>
+          <cell r="AB46">
+            <v>0.13133529282051357</v>
+          </cell>
+          <cell r="AC46">
+            <v>0.93188675055421044</v>
+          </cell>
+          <cell r="AD46">
+            <v>0.80055145773369685</v>
+          </cell>
+          <cell r="AE46">
+            <v>0.80055145773369685</v>
+          </cell>
+          <cell r="AF46">
+            <v>0.66921616491318325</v>
+          </cell>
+          <cell r="AG46">
+            <v>0.66921616491318325</v>
+          </cell>
+          <cell r="AH46">
+            <v>0.53788087209266966</v>
+          </cell>
         </row>
         <row r="47">
           <cell r="A47" t="str">
@@ -8176,6 +8224,54 @@
           <cell r="L47">
             <v>0.83625664580344583</v>
           </cell>
+          <cell r="S47">
+            <v>0.23644049244401955</v>
+          </cell>
+          <cell r="T47">
+            <v>7.8813497481339853E-2</v>
+          </cell>
+          <cell r="U47">
+            <v>0.59981615335942629</v>
+          </cell>
+          <cell r="V47">
+            <v>0.6786296508407661</v>
+          </cell>
+          <cell r="W47">
+            <v>0.6786296508407661</v>
+          </cell>
+          <cell r="X47">
+            <v>0.75744314832210591</v>
+          </cell>
+          <cell r="Y47">
+            <v>0.75744314832210591</v>
+          </cell>
+          <cell r="Z47">
+            <v>0.83625664580344572</v>
+          </cell>
+          <cell r="AA47">
+            <v>0.20190906716278284</v>
+          </cell>
+          <cell r="AB47">
+            <v>6.730302238759428E-2</v>
+          </cell>
+          <cell r="AC47">
+            <v>0.59981615335942629</v>
+          </cell>
+          <cell r="AD47">
+            <v>0.53251313097183206</v>
+          </cell>
+          <cell r="AE47">
+            <v>0.53251313097183206</v>
+          </cell>
+          <cell r="AF47">
+            <v>0.46521010858423778</v>
+          </cell>
+          <cell r="AG47">
+            <v>0.46521010858423778</v>
+          </cell>
+          <cell r="AH47">
+            <v>0.3979070861966435</v>
+          </cell>
         </row>
         <row r="48">
           <cell r="A48" t="str">
@@ -8213,6 +8309,54 @@
           </cell>
           <cell r="L48">
             <v>1.0532246400700302</v>
+          </cell>
+          <cell r="S48">
+            <v>0.28534277574146538</v>
+          </cell>
+          <cell r="T48">
+            <v>9.5114258580488456E-2</v>
+          </cell>
+          <cell r="U48">
+            <v>0.76788186432856487</v>
+          </cell>
+          <cell r="V48">
+            <v>0.86299612290905336</v>
+          </cell>
+          <cell r="W48">
+            <v>0.86299612290905336</v>
+          </cell>
+          <cell r="X48">
+            <v>0.95811038148954186</v>
+          </cell>
+          <cell r="Y48">
+            <v>0.95811038148954186</v>
+          </cell>
+          <cell r="Z48">
+            <v>1.0532246400700302</v>
+          </cell>
+          <cell r="AA48">
+            <v>0.20325260788810129</v>
+          </cell>
+          <cell r="AB48">
+            <v>6.7750869296033758E-2</v>
+          </cell>
+          <cell r="AC48">
+            <v>0.76788186432856487</v>
+          </cell>
+          <cell r="AD48">
+            <v>0.70013099503253107</v>
+          </cell>
+          <cell r="AE48">
+            <v>0.70013099503253107</v>
+          </cell>
+          <cell r="AF48">
+            <v>0.63238012573649727</v>
+          </cell>
+          <cell r="AG48">
+            <v>0.63238012573649727</v>
+          </cell>
+          <cell r="AH48">
+            <v>0.56462925644046347</v>
           </cell>
         </row>
       </sheetData>
@@ -11662,6 +11806,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19727,10 +19875,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9326B0-7C0C-4E7E-BEE0-B65D0C740685}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20794,6 +20942,204 @@
         <v>0.56462925644046347</v>
       </c>
     </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <f>[1]Weight23_24xRuns!S46</f>
+        <v>0.475724881892711</v>
+      </c>
+      <c r="B17" s="1">
+        <f>[1]Weight23_24xRuns!T46</f>
+        <v>0.15857496063090368</v>
+      </c>
+      <c r="C17" s="1">
+        <f>[1]Weight23_24xRuns!U46</f>
+        <v>0.93188675055421044</v>
+      </c>
+      <c r="D17" s="1">
+        <f>[1]Weight23_24xRuns!V46</f>
+        <v>1.090461711185114</v>
+      </c>
+      <c r="E17" s="1">
+        <f>[1]Weight23_24xRuns!W46</f>
+        <v>1.090461711185114</v>
+      </c>
+      <c r="F17" s="1">
+        <f>[1]Weight23_24xRuns!X46</f>
+        <v>1.2490366718160177</v>
+      </c>
+      <c r="G17" s="1">
+        <f>[1]Weight23_24xRuns!Y46</f>
+        <v>1.2490366718160177</v>
+      </c>
+      <c r="H17" s="1">
+        <f>[1]Weight23_24xRuns!Z46</f>
+        <v>1.4076116324469214</v>
+      </c>
+      <c r="I17" s="1">
+        <f>[1]Weight23_24xRuns!AA46</f>
+        <v>0.39400587846154067</v>
+      </c>
+      <c r="J17" s="1">
+        <f>[1]Weight23_24xRuns!AB46</f>
+        <v>0.13133529282051357</v>
+      </c>
+      <c r="K17" s="1">
+        <f>[1]Weight23_24xRuns!AC46</f>
+        <v>0.93188675055421044</v>
+      </c>
+      <c r="L17" s="1">
+        <f>[1]Weight23_24xRuns!AD46</f>
+        <v>0.80055145773369685</v>
+      </c>
+      <c r="M17" s="1">
+        <f>[1]Weight23_24xRuns!AE46</f>
+        <v>0.80055145773369685</v>
+      </c>
+      <c r="N17" s="1">
+        <f>[1]Weight23_24xRuns!AF46</f>
+        <v>0.66921616491318325</v>
+      </c>
+      <c r="O17" s="1">
+        <f>[1]Weight23_24xRuns!AG46</f>
+        <v>0.66921616491318325</v>
+      </c>
+      <c r="P17" s="1">
+        <f>[1]Weight23_24xRuns!AH46</f>
+        <v>0.53788087209266966</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <f>[1]Weight23_24xRuns!S47</f>
+        <v>0.23644049244401955</v>
+      </c>
+      <c r="B18" s="1">
+        <f>[1]Weight23_24xRuns!T47</f>
+        <v>7.8813497481339853E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <f>[1]Weight23_24xRuns!U47</f>
+        <v>0.59981615335942629</v>
+      </c>
+      <c r="D18" s="1">
+        <f>[1]Weight23_24xRuns!V47</f>
+        <v>0.6786296508407661</v>
+      </c>
+      <c r="E18" s="1">
+        <f>[1]Weight23_24xRuns!W47</f>
+        <v>0.6786296508407661</v>
+      </c>
+      <c r="F18" s="1">
+        <f>[1]Weight23_24xRuns!X47</f>
+        <v>0.75744314832210591</v>
+      </c>
+      <c r="G18" s="1">
+        <f>[1]Weight23_24xRuns!Y47</f>
+        <v>0.75744314832210591</v>
+      </c>
+      <c r="H18" s="1">
+        <f>[1]Weight23_24xRuns!Z47</f>
+        <v>0.83625664580344572</v>
+      </c>
+      <c r="I18" s="1">
+        <f>[1]Weight23_24xRuns!AA47</f>
+        <v>0.20190906716278284</v>
+      </c>
+      <c r="J18" s="1">
+        <f>[1]Weight23_24xRuns!AB47</f>
+        <v>6.730302238759428E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <f>[1]Weight23_24xRuns!AC47</f>
+        <v>0.59981615335942629</v>
+      </c>
+      <c r="L18" s="1">
+        <f>[1]Weight23_24xRuns!AD47</f>
+        <v>0.53251313097183206</v>
+      </c>
+      <c r="M18" s="1">
+        <f>[1]Weight23_24xRuns!AE47</f>
+        <v>0.53251313097183206</v>
+      </c>
+      <c r="N18" s="1">
+        <f>[1]Weight23_24xRuns!AF47</f>
+        <v>0.46521010858423778</v>
+      </c>
+      <c r="O18" s="1">
+        <f>[1]Weight23_24xRuns!AG47</f>
+        <v>0.46521010858423778</v>
+      </c>
+      <c r="P18" s="1">
+        <f>[1]Weight23_24xRuns!AH47</f>
+        <v>0.3979070861966435</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <f>[1]Weight23_24xRuns!S48</f>
+        <v>0.28534277574146538</v>
+      </c>
+      <c r="B19" s="1">
+        <f>[1]Weight23_24xRuns!T48</f>
+        <v>9.5114258580488456E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <f>[1]Weight23_24xRuns!U48</f>
+        <v>0.76788186432856487</v>
+      </c>
+      <c r="D19" s="1">
+        <f>[1]Weight23_24xRuns!V48</f>
+        <v>0.86299612290905336</v>
+      </c>
+      <c r="E19" s="1">
+        <f>[1]Weight23_24xRuns!W48</f>
+        <v>0.86299612290905336</v>
+      </c>
+      <c r="F19" s="1">
+        <f>[1]Weight23_24xRuns!X48</f>
+        <v>0.95811038148954186</v>
+      </c>
+      <c r="G19" s="1">
+        <f>[1]Weight23_24xRuns!Y48</f>
+        <v>0.95811038148954186</v>
+      </c>
+      <c r="H19" s="1">
+        <f>[1]Weight23_24xRuns!Z48</f>
+        <v>1.0532246400700302</v>
+      </c>
+      <c r="I19" s="1">
+        <f>[1]Weight23_24xRuns!AA48</f>
+        <v>0.20325260788810129</v>
+      </c>
+      <c r="J19" s="1">
+        <f>[1]Weight23_24xRuns!AB48</f>
+        <v>6.7750869296033758E-2</v>
+      </c>
+      <c r="K19" s="1">
+        <f>[1]Weight23_24xRuns!AC48</f>
+        <v>0.76788186432856487</v>
+      </c>
+      <c r="L19" s="1">
+        <f>[1]Weight23_24xRuns!AD48</f>
+        <v>0.70013099503253107</v>
+      </c>
+      <c r="M19" s="1">
+        <f>[1]Weight23_24xRuns!AE48</f>
+        <v>0.70013099503253107</v>
+      </c>
+      <c r="N19" s="1">
+        <f>[1]Weight23_24xRuns!AF48</f>
+        <v>0.63238012573649727</v>
+      </c>
+      <c r="O19" s="1">
+        <f>[1]Weight23_24xRuns!AG48</f>
+        <v>0.63238012573649727</v>
+      </c>
+      <c r="P19" s="1">
+        <f>[1]Weight23_24xRuns!AH48</f>
+        <v>0.56462925644046347</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20801,10 +21147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CF4723-4815-492D-AAD5-13AA3CB4155F}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21361,6 +21707,9 @@
         <f>[1]Weight23_24Probs!M26</f>
         <v>0.29978048609077712</v>
       </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26877,7 +27226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B11C03A-EFA1-4924-BD4E-E8F8DD3A901F}">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>

</xml_diff>